<commit_message>
Added code to handle the possible pop-up window that there are open quotations.
</commit_message>
<xml_diff>
--- a/SAPGUI_VA01_Create_New_Sales_Order/Default.xlsx
+++ b/SAPGUI_VA01_Create_New_Sales_Order/Default.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Action1" sheetId="2" r:id="rId2"/>
+    <sheet name="VA01" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -493,7 +493,9 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>

</xml_diff>

<commit_message>
Updated to have a fourth example of using the output value, this time with the RUNTIME datatable.
</commit_message>
<xml_diff>
--- a/SAPGUI_VA01_Create_New_Sales_Order/Default.xlsx
+++ b/SAPGUI_VA01_Create_New_Sales_Order/Default.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+  <si>
+    <t>dtOrderNumber</t>
+  </si>
   <si>
     <t>StatusBar_item2_out</t>
   </si>
@@ -162,12 +165,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -187,12 +201,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -491,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -500,10 +517,14 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="18.6015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
+      <c t="s">
+        <v>1</v>
+      </c>
       <c t="s">
         <v>0</v>
       </c>
@@ -512,6 +533,7 @@
       <c s="2">
         <v>12925</v>
       </c>
+      <c s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>